<commit_message>
Add toliatti, old json_maker for all regions
</commit_message>
<xml_diff>
--- a/xlsx/nsk.xlsx
+++ b/xlsx/nsk.xlsx
@@ -7151,11 +7151,11 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>1699000</v>
+        <v>1709400</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>https://sib-autosalon.ru/cars/haval/new_f7/</t>
+          <t>https://centorauto-nsk.ru/avto-new/haval/haval_f7_%D0%BD%D0%BE%D0%B2%D1%8B%D0%B9/</t>
         </is>
       </c>
       <c r="F116" t="n">
@@ -7167,11 +7167,11 @@
         </is>
       </c>
       <c r="L116" t="n">
-        <v>1699000</v>
+        <v>1979000</v>
       </c>
       <c r="M116" t="inlineStr">
         <is>
-          <t>https://sib-autosalon.ru/cars/haval/new_f7/</t>
+          <t>https://sib-autosalon.ru/cars/haval/f7_ii/</t>
         </is>
       </c>
       <c r="N116" t="n">

</xml_diff>